<commit_message>
Update Reference TANF & SSP WPR & TL Feedback Reports.xlsx
</commit_message>
<xml_diff>
--- a/knowledge-center/Reference TANF & SSP WPR & TL Feedback Reports.xlsx
+++ b/knowledge-center/Reference TANF & SSP WPR & TL Feedback Reports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29728"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hhsgov-my.sharepoint.com/personal/yun_song_acf_hhs_gov/Documents/Documents/PR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C575B1-727F-4E17-B482-E88569739B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD6F4470-9F00-43D6-87CF-B0FAA6EEEA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7827,8 +7827,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F80BF35C5C40419CB0899C34EDCF7D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ad2f5140b36ed19d8ca0706ec53391d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9eaf715c-9c82-42ca-98d9-220ae20560c2" xmlns:ns3="950ef47f-4b71-4db6-a5e7-27137d313915" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b981160422772e641471dd46bcf534aa" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9eaf715c-9c82-42ca-98d9-220ae20560c2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="950ef47f-4b71-4db6-a5e7-27137d313915">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F80BF35C5C40419CB0899C34EDCF7D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15722ed76ccbde7256eeb804f6fd52d8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9eaf715c-9c82-42ca-98d9-220ae20560c2" xmlns:ns3="950ef47f-4b71-4db6-a5e7-27137d313915" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a8188ae6d014953ae15a8015499b11ef" ns2:_="" ns3:_="">
     <xsd:import namespace="9eaf715c-9c82-42ca-98d9-220ae20560c2"/>
     <xsd:import namespace="950ef47f-4b71-4db6-a5e7-27137d313915"/>
     <xsd:element name="properties">
@@ -8055,7 +8066,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8064,27 +8075,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9eaf715c-9c82-42ca-98d9-220ae20560c2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="950ef47f-4b71-4db6-a5e7-27137d313915">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D835F615-2251-4298-8433-2230927A7279}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E919274E-B1E5-44E4-B80C-4EE7385A1ADE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FA57A7-F82A-464A-A112-5685B0F11090}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C970BC8-C7D0-4CA8-B93E-0D34DDF640B1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E919274E-B1E5-44E4-B80C-4EE7385A1ADE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11FA57A7-F82A-464A-A112-5685B0F11090}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>